<commit_message>
Latest set of changes - still need to address admin registration flow
</commit_message>
<xml_diff>
--- a/appGreece/config/assets/framework/forms/framework/framework.xlsx
+++ b/appGreece/config/assets/framework/forms/framework/framework.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/app/config/assets/framework/forms/framework/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="2260" windowWidth="24660" windowHeight="17960" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="16920" yWindow="1900" windowWidth="24660" windowHeight="17960" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -19,13 +14,13 @@
     <sheet name="choices" sheetId="5" r:id="rId5"/>
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="307">
   <si>
     <t>comments</t>
   </si>
@@ -113,15 +108,6 @@
   </si>
   <si>
     <t>text.spanish</t>
-  </si>
-  <si>
-    <t>select_user</t>
-  </si>
-  <si>
-    <t>Please Select User</t>
-  </si>
-  <si>
-    <t>Seleccione usuario</t>
   </si>
   <si>
     <t>main_title</t>
@@ -944,6 +930,39 @@
   </si>
   <si>
     <t>search_beneficiaries</t>
+  </si>
+  <si>
+    <t>view_household_data</t>
+  </si>
+  <si>
+    <t>View Household Data</t>
+  </si>
+  <si>
+    <t>active_households</t>
+  </si>
+  <si>
+    <t>Active Households</t>
+  </si>
+  <si>
+    <t>disabled_households</t>
+  </si>
+  <si>
+    <t>Disabled Households</t>
+  </si>
+  <si>
+    <t>household_data</t>
+  </si>
+  <si>
+    <t>Household Data</t>
+  </si>
+  <si>
+    <t>Seleccione grupo</t>
+  </si>
+  <si>
+    <t>Please Select Group</t>
+  </si>
+  <si>
+    <t>select_group</t>
   </si>
 </sst>
 </file>
@@ -1388,7 +1407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1402,9 +1421,9 @@
       <selection activeCell="B23" activeCellId="1" sqref="B87 B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1420,6 +1439,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1431,7 +1455,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
@@ -1442,7 +1466,7 @@
     <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1469,7 +1493,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="39" customHeight="1">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -1478,7 +1502,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -1489,13 +1513,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -1506,26 +1530,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -1534,23 +1558,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1559,7 +1583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" t="s">
@@ -1569,24 +1593,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="41" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1597,495 +1627,532 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13">
+      <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>45</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
         <v>47</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>54</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>57</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>59</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>66</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
         <v>68</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="52" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>74</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>75</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>78</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
         <v>80</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
+      <c r="B22" t="s">
         <v>83</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
         <v>85</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
         <v>87</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
         <v>89</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+      <c r="B26" t="s">
         <v>91</v>
       </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
         <v>93</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
         <v>95</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
         <v>97</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
         <v>101</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
         <v>103</v>
       </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
         <v>105</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
+      <c r="B34" t="s">
         <v>107</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
         <v>109</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
+      <c r="B36" t="s">
         <v>111</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
         <v>113</v>
       </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
+      <c r="B38" t="s">
         <v>115</v>
       </c>
-      <c r="B37" t="s">
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
+      <c r="B39" t="s">
         <v>117</v>
       </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>295</v>
+      </c>
+      <c r="B40" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>119</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" s="2" customFormat="1">
+      <c r="A53" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
-        <v>124</v>
-      </c>
-      <c r="B42" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
-        <v>125</v>
-      </c>
-      <c r="B43" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
-        <v>126</v>
-      </c>
-      <c r="B44" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
-        <v>128</v>
-      </c>
-      <c r="B46" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
-        <v>129</v>
-      </c>
-      <c r="B47" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A52" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>292</v>
+      <c r="B56" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2097,46 +2164,46 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" t="s">
         <v>146</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>147</v>
-      </c>
-      <c r="F1" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H1" t="s">
-        <v>150</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
       </c>
       <c r="J1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2145,12 +2212,12 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2159,113 +2226,118 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="I4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28" customHeight="1">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+      <c r="I5" t="s">
         <v>158</v>
-      </c>
-      <c r="C5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" t="s">
-        <v>159</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="I5" t="s">
-        <v>161</v>
       </c>
       <c r="J5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1">
       <c r="A7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" t="s">
         <v>162</v>
       </c>
-      <c r="F7" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A8" t="s">
         <v>163</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F8" t="s">
         <v>164</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1">
+      <c r="A9" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="F8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G8" t="s">
-        <v>167</v>
-      </c>
-      <c r="H8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2277,49 +2349,54 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2331,13 +2408,13 @@
       <selection activeCellId="1" sqref="B87 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="13" customHeight="1">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2345,466 +2422,471 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13" customHeight="1">
+      <c r="A2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="13" customHeight="1">
+      <c r="A3" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>179</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="13" customHeight="1">
+      <c r="A4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>181</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="13" customHeight="1">
+      <c r="A5" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>183</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="13" customHeight="1">
+      <c r="A6" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>185</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="13">
+      <c r="A7" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>187</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" ht="13">
+      <c r="A8" t="s">
         <v>189</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" ht="13">
+      <c r="A9" t="s">
         <v>192</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" ht="13">
+      <c r="A10" t="s">
         <v>195</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>196</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" ht="13.75" customHeight="1">
+      <c r="A11" t="s">
         <v>198</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>199</v>
       </c>
-      <c r="C10" s="6" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="13.75" customHeight="1">
+      <c r="A12" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
         <v>201</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
         <v>203</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
         <v>205</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
         <v>207</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
         <v>209</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
         <v>211</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
         <v>213</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
         <v>215</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
         <v>217</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
         <v>219</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
+      <c r="B22" t="s">
         <v>221</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
         <v>223</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
         <v>225</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
+      <c r="B25" t="s">
         <v>227</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+      <c r="B26" t="s">
         <v>229</v>
       </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
+      <c r="B27" t="s">
         <v>231</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="28.25" customHeight="1">
+      <c r="A28" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
+      <c r="B28" t="s">
         <v>233</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
+      <c r="B29" t="s">
         <v>235</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
         <v>237</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
         <v>239</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
+      <c r="B33" t="s">
         <v>241</v>
       </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" t="s">
+      <c r="B34" t="s">
         <v>243</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
         <v>245</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="409">
+      <c r="A36" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
+      <c r="B36" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="409" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
         <v>249</v>
       </c>
-      <c r="B36" s="3" t="s">
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
+      <c r="B38" t="s">
         <v>251</v>
       </c>
-      <c r="B37" t="s">
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" t="s">
+      <c r="B39" t="s">
         <v>253</v>
       </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" t="s">
+      <c r="B40" t="s">
         <v>255</v>
       </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
         <v>257</v>
       </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" t="s">
+      <c r="B42" t="s">
         <v>259</v>
       </c>
-      <c r="B41" t="s">
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" t="s">
+      <c r="B43" t="s">
         <v>261</v>
       </c>
-      <c r="B42" t="s">
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" t="s">
+      <c r="B44" t="s">
         <v>263</v>
       </c>
-      <c r="B43" t="s">
+    </row>
+    <row r="45" spans="1:3" ht="13">
+      <c r="A45" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
+      <c r="B45" t="s">
         <v>265</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C45" s="6" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
         <v>267</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>268</v>
       </c>
-      <c r="C45" s="6" t="s">
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
+      <c r="B47" t="s">
         <v>270</v>
       </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
+      <c r="B48" t="s">
         <v>272</v>
       </c>
-      <c r="B47" t="s">
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
+      <c r="B49" t="s">
         <v>274</v>
       </c>
-      <c r="B48" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="13" customHeight="1">
+      <c r="A50" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
+      <c r="B50" t="s">
         <v>276</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
+      <c r="B51" t="s">
         <v>278</v>
       </c>
-      <c r="B50" t="s">
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
+      <c r="B52" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>280</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
         <v>282</v>
       </c>
-      <c r="B52" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" t="s">
+      <c r="B54" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>283</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
+      <c r="B56" t="s">
         <v>285</v>
       </c>
-      <c r="B54" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A55" t="s">
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
         <v>286</v>
       </c>
-      <c r="B55" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
+      <c r="B57" t="s">
         <v>287</v>
-      </c>
-      <c r="B56" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
-        <v>289</v>
-      </c>
-      <c r="B57" t="s">
-        <v>290</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add select_group translation back in
</commit_message>
<xml_diff>
--- a/appGreece/config/assets/framework/forms/framework/framework.xlsx
+++ b/appGreece/config/assets/framework/forms/framework/framework.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/assets/framework/forms/framework/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27820" yWindow="14460" windowWidth="31660" windowHeight="16880" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="8700" yWindow="0" windowWidth="28940" windowHeight="22520" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -19,13 +14,13 @@
     <sheet name="choices" sheetId="5" r:id="rId5"/>
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="679">
   <si>
     <t>comments</t>
   </si>
@@ -2078,6 +2073,12 @@
   </si>
   <si>
     <t>Household Advanced Search</t>
+  </si>
+  <si>
+    <t>select_group</t>
+  </si>
+  <si>
+    <t>Please Select Group</t>
   </si>
 </sst>
 </file>
@@ -2140,8 +2141,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2169,11 +2172,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2509,7 +2514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2523,9 +2528,9 @@
       <selection activeCell="B23" activeCellId="1" sqref="B87 B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2541,6 +2546,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2552,7 +2562,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
@@ -2563,7 +2573,7 @@
     <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2590,7 +2600,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="39" customHeight="1">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -2599,7 +2609,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -2610,13 +2620,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -2627,23 +2637,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
         <v>256</v>
@@ -2655,20 +2665,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
         <v>257</v>
@@ -2680,7 +2690,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" t="s">
@@ -2690,18 +2700,23 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="3" width="49.5" customWidth="1"/>
@@ -2709,7 +2724,7 @@
     <col min="5" max="7" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2732,7 +2747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2755,7 +2770,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2778,7 +2793,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2801,7 +2816,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2824,7 +2839,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2847,7 +2862,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -2870,7 +2885,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2893,7 +2908,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2916,7 +2931,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2939,7 +2954,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2962,7 +2977,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2985,7 +3000,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3008,7 +3023,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3031,7 +3046,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="34">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3054,7 +3069,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -3077,7 +3092,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3100,7 +3115,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3123,7 +3138,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3146,7 +3161,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -3169,7 +3184,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -3192,7 +3207,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -3215,7 +3230,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -3238,7 +3253,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -3261,7 +3276,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -3284,7 +3299,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -3307,7 +3322,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -3330,7 +3345,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -3353,7 +3368,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -3376,7 +3391,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -3399,7 +3414,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -3422,7 +3437,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -3445,7 +3460,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3468,7 +3483,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -3491,7 +3506,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -3514,7 +3529,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -3537,7 +3552,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -3560,7 +3575,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3583,7 +3598,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -3606,7 +3621,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>259</v>
       </c>
@@ -3629,7 +3644,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -3652,7 +3667,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>107</v>
       </c>
@@ -3675,7 +3690,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -3698,7 +3713,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -3721,7 +3736,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>110</v>
       </c>
@@ -3744,7 +3759,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>111</v>
       </c>
@@ -3767,7 +3782,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>112</v>
       </c>
@@ -3790,7 +3805,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3813,7 +3828,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" s="2" t="s">
         <v>115</v>
       </c>
@@ -3836,7 +3851,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" s="2" t="s">
         <v>116</v>
       </c>
@@ -3859,7 +3874,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="36" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="34">
       <c r="A51" s="2" t="s">
         <v>118</v>
       </c>
@@ -3882,7 +3897,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" s="2" t="s">
         <v>120</v>
       </c>
@@ -3905,7 +3920,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" s="2" customFormat="1">
       <c r="A53" s="2" t="s">
         <v>122</v>
       </c>
@@ -3928,7 +3943,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
         <v>253</v>
       </c>
@@ -3951,7 +3966,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" s="2" t="s">
         <v>665</v>
       </c>
@@ -3961,7 +3976,7 @@
       <c r="C55" s="5"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" s="2" t="s">
         <v>667</v>
       </c>
@@ -3969,7 +3984,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" s="2" t="s">
         <v>669</v>
       </c>
@@ -3977,7 +3992,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
         <v>671</v>
       </c>
@@ -3985,7 +4000,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
         <v>673</v>
       </c>
@@ -3993,7 +4008,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" s="2" t="s">
         <v>674</v>
       </c>
@@ -4001,9 +4016,25 @@
         <v>676</v>
       </c>
     </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>677</v>
+      </c>
+      <c r="B61" t="s">
+        <v>678</v>
+      </c>
+      <c r="C61" t="s">
+        <v>678</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4015,9 +4046,9 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
@@ -4061,7 +4092,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>131</v>
       </c>
@@ -4079,7 +4110,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -4100,7 +4131,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
@@ -4111,7 +4142,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" ht="28" customHeight="1">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4138,7 +4169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -4158,7 +4189,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>143</v>
       </c>
@@ -4184,7 +4215,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>660</v>
       </c>
@@ -4210,7 +4241,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>661</v>
       </c>
@@ -4236,7 +4267,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -4262,7 +4293,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -4270,6 +4301,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4281,14 +4317,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -4299,7 +4335,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -4310,7 +4346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -4324,6 +4360,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4335,13 +4376,13 @@
       <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="2" max="2" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="13" customHeight="1">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -4361,7 +4402,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13" customHeight="1">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -4381,7 +4422,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="13" customHeight="1">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -4401,7 +4442,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="13" customHeight="1">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -4421,7 +4462,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="13" customHeight="1">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -4441,7 +4482,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="13" customHeight="1">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -4461,7 +4502,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="17">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -4481,7 +4522,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="17">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -4501,7 +4542,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -4521,7 +4562,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="17">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -4541,7 +4582,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="13.75" customHeight="1">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -4561,7 +4602,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="13.75" customHeight="1">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -4581,7 +4622,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="17">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -4601,7 +4642,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="17">
       <c r="A14" t="s">
         <v>175</v>
       </c>
@@ -4621,7 +4662,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="17">
       <c r="A15" t="s">
         <v>177</v>
       </c>
@@ -4641,7 +4682,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="17">
       <c r="A16" t="s">
         <v>179</v>
       </c>
@@ -4661,7 +4702,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="17">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -4681,7 +4722,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17">
       <c r="A18" t="s">
         <v>183</v>
       </c>
@@ -4701,7 +4742,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="17">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -4721,7 +4762,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="17">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -4741,7 +4782,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="17">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -4761,7 +4802,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="17">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -4781,7 +4822,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="17">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -4801,7 +4842,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="17">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -4821,7 +4862,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="17">
       <c r="A25" t="s">
         <v>197</v>
       </c>
@@ -4841,7 +4882,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="17">
       <c r="A26" t="s">
         <v>199</v>
       </c>
@@ -4861,7 +4902,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="17">
       <c r="A27" t="s">
         <v>201</v>
       </c>
@@ -4881,7 +4922,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="28.25" customHeight="1">
       <c r="A28" t="s">
         <v>203</v>
       </c>
@@ -4893,7 +4934,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="17">
       <c r="A29" t="s">
         <v>205</v>
       </c>
@@ -4905,7 +4946,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="17">
       <c r="A30" t="s">
         <v>207</v>
       </c>
@@ -4925,7 +4966,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="17">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -4945,13 +4986,13 @@
         <v>485</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="17">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="17">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -4971,7 +5012,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="17">
       <c r="A34" t="s">
         <v>213</v>
       </c>
@@ -4991,7 +5032,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="17">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -5011,7 +5052,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="157">
       <c r="A36" t="s">
         <v>217</v>
       </c>
@@ -5023,7 +5064,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="17">
       <c r="A37" t="s">
         <v>219</v>
       </c>
@@ -5043,7 +5084,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="17">
       <c r="A38" t="s">
         <v>221</v>
       </c>
@@ -5063,7 +5104,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="17">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5083,7 +5124,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="17">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5103,7 +5144,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="17">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5123,7 +5164,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="17">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5143,7 +5184,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="17">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5163,7 +5204,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="17">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5183,7 +5224,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="17">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5203,7 +5244,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="17">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5223,7 +5264,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="17">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5243,7 +5284,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="17">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5263,7 +5304,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="17">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5283,7 +5324,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="13" customHeight="1">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -5303,7 +5344,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="17">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -5323,7 +5364,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="17">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -5343,7 +5384,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="17">
       <c r="A53" t="s">
         <v>250</v>
       </c>
@@ -5363,7 +5404,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="17">
       <c r="A54" t="s">
         <v>252</v>
       </c>
@@ -5383,64 +5424,69 @@
         <v>526</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="17">
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
     </row>
-    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="17">
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="17">
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="17">
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="17">
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="17">
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="17">
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="17">
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="17">
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="17">
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" spans="3:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:4" ht="17">
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
     </row>
-    <row r="66" spans="3:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:4" ht="17">
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" spans="3:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:4" ht="17">
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
     </row>
-    <row r="68" spans="3:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:4" ht="17">
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
readd common survey translations
</commit_message>
<xml_diff>
--- a/appGreece/config/assets/framework/forms/framework/framework.xlsx
+++ b/appGreece/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/assets/framework/forms/framework/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="0" windowWidth="28940" windowHeight="22520" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="-27820" yWindow="14460" windowWidth="31660" windowHeight="16880" tabRatio="989" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -14,13 +19,13 @@
     <sheet name="choices" sheetId="5" r:id="rId5"/>
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="687">
   <si>
     <t>comments</t>
   </si>
@@ -2075,10 +2080,34 @@
     <t>Household Advanced Search</t>
   </si>
   <si>
-    <t>select_group</t>
-  </si>
-  <si>
-    <t>Please Select Group</t>
+    <t>barcode_button_label</t>
+  </si>
+  <si>
+    <t>invalid_numeric_message</t>
+  </si>
+  <si>
+    <t>Numeric value expected</t>
+  </si>
+  <si>
+    <t>invalid_integer_message</t>
+  </si>
+  <si>
+    <t>Integer value expected</t>
+  </si>
+  <si>
+    <t>Escanear Código de Barras</t>
+  </si>
+  <si>
+    <t>Valor numérico esperado</t>
+  </si>
+  <si>
+    <t>Valor entero esperado</t>
+  </si>
+  <si>
+    <t>Αναμενόμενη αριθμητική τιμή</t>
+  </si>
+  <si>
+    <t>Αναμενόμενη τιμή ακέραιας</t>
   </si>
 </sst>
 </file>
@@ -2141,16 +2170,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2171,14 +2198,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2514,7 +2542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2528,9 +2556,9 @@
       <selection activeCell="B23" activeCellId="1" sqref="B87 B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2538,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2546,11 +2574,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2562,7 +2585,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
@@ -2573,7 +2596,7 @@
     <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2600,7 +2623,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1">
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -2609,7 +2632,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -2620,13 +2643,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -2637,23 +2660,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
         <v>256</v>
@@ -2665,20 +2688,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
         <v>257</v>
@@ -2690,7 +2713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" t="s">
@@ -2700,23 +2723,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41:I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="3" width="49.5" customWidth="1"/>
@@ -2724,7 +2742,7 @@
     <col min="5" max="7" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2747,7 +2765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2770,7 +2788,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2793,7 +2811,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2816,7 +2834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2839,7 +2857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2862,7 +2880,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -2885,7 +2903,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2908,7 +2926,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2931,7 +2949,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2954,7 +2972,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2977,7 +2995,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -3000,7 +3018,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3023,7 +3041,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3046,7 +3064,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="34">
+    <row r="15" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3069,7 +3087,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -3092,7 +3110,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3115,7 +3133,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3138,7 +3156,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3161,7 +3179,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -3184,7 +3202,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -3207,7 +3225,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -3230,7 +3248,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -3253,7 +3271,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -3276,7 +3294,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -3299,7 +3317,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -3322,7 +3340,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -3345,7 +3363,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -3368,7 +3386,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -3391,7 +3409,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -3414,7 +3432,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -3437,7 +3455,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -3460,7 +3478,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3483,7 +3501,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -3506,7 +3524,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -3529,7 +3547,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -3552,7 +3570,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -3575,7 +3593,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3598,7 +3616,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -3621,7 +3639,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>259</v>
       </c>
@@ -3644,7 +3662,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -3667,7 +3685,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>107</v>
       </c>
@@ -3690,7 +3708,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -3713,7 +3731,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -3736,7 +3754,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>110</v>
       </c>
@@ -3759,7 +3777,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>111</v>
       </c>
@@ -3782,7 +3800,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>112</v>
       </c>
@@ -3805,7 +3823,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3828,7 +3846,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>115</v>
       </c>
@@ -3851,7 +3869,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>116</v>
       </c>
@@ -3874,7 +3892,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="34">
+    <row r="51" spans="1:7" ht="36" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>118</v>
       </c>
@@ -3897,7 +3915,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>120</v>
       </c>
@@ -3920,7 +3938,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="2" customFormat="1">
+    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>122</v>
       </c>
@@ -3943,7 +3961,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>253</v>
       </c>
@@ -3966,7 +3984,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>665</v>
       </c>
@@ -3976,7 +3994,7 @@
       <c r="C55" s="5"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>667</v>
       </c>
@@ -3984,7 +4002,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>669</v>
       </c>
@@ -3992,7 +4010,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>671</v>
       </c>
@@ -4000,7 +4018,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>673</v>
       </c>
@@ -4008,7 +4026,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>674</v>
       </c>
@@ -4016,25 +4034,9 @@
         <v>676</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
-      <c r="A61" t="s">
-        <v>677</v>
-      </c>
-      <c r="B61" t="s">
-        <v>678</v>
-      </c>
-      <c r="C61" t="s">
-        <v>678</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -4046,9 +4048,9 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
@@ -4092,7 +4094,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>131</v>
       </c>
@@ -4110,7 +4112,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -4131,7 +4133,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
@@ -4142,7 +4144,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28" customHeight="1">
+    <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4169,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -4189,7 +4191,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>143</v>
       </c>
@@ -4215,7 +4217,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>660</v>
       </c>
@@ -4241,7 +4243,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>661</v>
       </c>
@@ -4267,7 +4269,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -4293,7 +4295,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -4301,11 +4303,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4317,14 +4314,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -4335,7 +4332,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -4346,7 +4343,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -4360,11 +4357,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4372,17 +4364,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="2" max="2" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" customHeight="1">
+    <row r="1" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -4402,7 +4394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13" customHeight="1">
+    <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -4422,7 +4414,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13" customHeight="1">
+    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -4442,7 +4434,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13" customHeight="1">
+    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -4462,7 +4454,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13" customHeight="1">
+    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -4482,7 +4474,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13" customHeight="1">
+    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -4502,7 +4494,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -4522,7 +4514,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -4542,7 +4534,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -4562,7 +4554,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -4582,7 +4574,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.75" customHeight="1">
+    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -4602,7 +4594,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.75" customHeight="1">
+    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -4622,7 +4614,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17">
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -4642,7 +4634,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>175</v>
       </c>
@@ -4662,7 +4654,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>177</v>
       </c>
@@ -4682,7 +4674,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17">
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>179</v>
       </c>
@@ -4702,7 +4694,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17">
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -4722,7 +4714,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17">
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>183</v>
       </c>
@@ -4742,7 +4734,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17">
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -4762,7 +4754,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17">
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -4782,7 +4774,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17">
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -4802,7 +4794,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17">
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -4822,7 +4814,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17">
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -4842,7 +4834,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17">
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -4862,7 +4854,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17">
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>197</v>
       </c>
@@ -4882,7 +4874,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17">
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>199</v>
       </c>
@@ -4902,7 +4894,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17">
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>201</v>
       </c>
@@ -4922,7 +4914,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.25" customHeight="1">
+    <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>203</v>
       </c>
@@ -4934,7 +4926,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="17">
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>205</v>
       </c>
@@ -4946,7 +4938,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="17">
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>207</v>
       </c>
@@ -4966,7 +4958,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17">
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -4986,13 +4978,13 @@
         <v>485</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17">
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="17">
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -5012,7 +5004,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17">
+    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>213</v>
       </c>
@@ -5032,7 +5024,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17">
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -5052,7 +5044,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="157">
+    <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>217</v>
       </c>
@@ -5064,7 +5056,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="17">
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>219</v>
       </c>
@@ -5084,7 +5076,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17">
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>221</v>
       </c>
@@ -5104,7 +5096,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17">
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5124,7 +5116,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="17">
+    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5144,7 +5136,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17">
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5164,7 +5156,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="17">
+    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5184,7 +5176,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="17">
+    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5204,7 +5196,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17">
+    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5224,7 +5216,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17">
+    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5244,7 +5236,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="17">
+    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5264,7 +5256,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="17">
+    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5284,7 +5276,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17">
+    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5304,7 +5296,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="17">
+    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5324,7 +5316,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13" customHeight="1">
+    <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -5344,7 +5336,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="17">
+    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -5364,7 +5356,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17">
+    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -5384,7 +5376,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="17">
+    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>250</v>
       </c>
@@ -5404,7 +5396,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="17">
+    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>252</v>
       </c>
@@ -5424,69 +5416,97 @@
         <v>526</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="17">
-      <c r="C55" s="5"/>
+    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="D55" s="5"/>
-    </row>
-    <row r="56" spans="1:6" ht="17">
-      <c r="C56" s="5"/>
+      <c r="F55" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>685</v>
+      </c>
       <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="1:6" ht="17">
-      <c r="C57" s="5"/>
+      <c r="F56" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>686</v>
+      </c>
       <c r="D57" s="5"/>
-    </row>
-    <row r="58" spans="1:6" ht="17">
+      <c r="F57" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:6" ht="17">
+    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:6" ht="17">
+    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:6" ht="17">
+    <row r="61" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:6" ht="17">
+    <row r="62" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="1:6" ht="17">
+    <row r="63" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" spans="1:6" ht="17">
+    <row r="64" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" spans="3:4" ht="17">
+    <row r="65" spans="3:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
     </row>
-    <row r="66" spans="3:4" ht="17">
+    <row r="66" spans="3:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" spans="3:4" ht="17">
+    <row r="67" spans="3:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
     </row>
-    <row r="68" spans="3:4" ht="17">
+    <row r="68" spans="3:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
select_group not showing up
</commit_message>
<xml_diff>
--- a/appGreece/config/assets/framework/forms/framework/framework.xlsx
+++ b/appGreece/config/assets/framework/forms/framework/framework.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/assets/framework/forms/framework/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27820" yWindow="14460" windowWidth="31660" windowHeight="16880" tabRatio="989" activeTab="5"/>
+    <workbookView xWindow="11280" yWindow="2560" windowWidth="29580" windowHeight="19960" tabRatio="989" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -19,13 +14,13 @@
     <sheet name="choices" sheetId="5" r:id="rId5"/>
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="689">
   <si>
     <t>comments</t>
   </si>
@@ -2108,6 +2103,12 @@
   </si>
   <si>
     <t>Αναμενόμενη τιμή ακέραιας</t>
+  </si>
+  <si>
+    <t>select_group</t>
+  </si>
+  <si>
+    <t>Please Select Group</t>
   </si>
 </sst>
 </file>
@@ -2170,8 +2171,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2202,11 +2205,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2542,7 +2547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2556,9 +2561,9 @@
       <selection activeCell="B23" activeCellId="1" sqref="B87 B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2566,7 +2571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2574,6 +2579,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2585,7 +2595,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
@@ -2596,7 +2606,7 @@
     <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2623,7 +2633,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="39" customHeight="1">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -2632,7 +2642,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -2643,13 +2653,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -2660,23 +2670,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
         <v>256</v>
@@ -2688,20 +2698,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
         <v>257</v>
@@ -2713,7 +2723,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" t="s">
@@ -2723,6 +2733,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2734,7 +2749,7 @@
       <selection activeCell="H41" sqref="H41:I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="3" width="49.5" customWidth="1"/>
@@ -2742,7 +2757,7 @@
     <col min="5" max="7" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2765,7 +2780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2788,7 +2803,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2811,7 +2826,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2834,7 +2849,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2857,7 +2872,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2880,7 +2895,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -2903,7 +2918,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2926,7 +2941,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -2949,7 +2964,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2972,7 +2987,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -2995,7 +3010,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -3018,7 +3033,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3041,7 +3056,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -3064,7 +3079,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="34">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -3087,7 +3102,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -3110,7 +3125,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3133,7 +3148,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -3156,7 +3171,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3179,7 +3194,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -3202,7 +3217,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -3225,7 +3240,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -3248,7 +3263,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -3271,7 +3286,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -3294,7 +3309,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -3317,7 +3332,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -3340,7 +3355,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -3363,7 +3378,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -3386,7 +3401,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -3409,7 +3424,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -3432,7 +3447,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -3455,7 +3470,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -3478,7 +3493,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3501,7 +3516,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -3524,7 +3539,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -3547,7 +3562,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -3570,7 +3585,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -3593,7 +3608,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -3616,7 +3631,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -3639,7 +3654,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>259</v>
       </c>
@@ -3662,7 +3677,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -3685,7 +3700,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>107</v>
       </c>
@@ -3708,7 +3723,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>108</v>
       </c>
@@ -3731,7 +3746,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>109</v>
       </c>
@@ -3754,7 +3769,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>110</v>
       </c>
@@ -3777,7 +3792,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>111</v>
       </c>
@@ -3800,7 +3815,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>112</v>
       </c>
@@ -3823,7 +3838,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" s="2" t="s">
         <v>114</v>
       </c>
@@ -3846,7 +3861,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" s="2" t="s">
         <v>115</v>
       </c>
@@ -3869,7 +3884,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" s="2" t="s">
         <v>116</v>
       </c>
@@ -3892,7 +3907,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="36" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="34">
       <c r="A51" s="2" t="s">
         <v>118</v>
       </c>
@@ -3915,7 +3930,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" s="2" t="s">
         <v>120</v>
       </c>
@@ -3938,7 +3953,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" s="2" customFormat="1">
       <c r="A53" s="2" t="s">
         <v>122</v>
       </c>
@@ -3961,7 +3976,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" s="2" t="s">
         <v>253</v>
       </c>
@@ -3984,7 +3999,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" s="2" t="s">
         <v>665</v>
       </c>
@@ -3994,7 +4009,7 @@
       <c r="C55" s="5"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" s="2" t="s">
         <v>667</v>
       </c>
@@ -4002,7 +4017,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" s="2" t="s">
         <v>669</v>
       </c>
@@ -4010,7 +4025,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" s="2" t="s">
         <v>671</v>
       </c>
@@ -4018,7 +4033,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" s="2" t="s">
         <v>673</v>
       </c>
@@ -4026,7 +4041,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" s="2" t="s">
         <v>674</v>
       </c>
@@ -4037,6 +4052,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4048,9 +4068,9 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
@@ -4094,7 +4114,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>131</v>
       </c>
@@ -4112,7 +4132,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -4133,7 +4153,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
@@ -4144,7 +4164,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" ht="28" customHeight="1">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4171,7 +4191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -4191,7 +4211,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>143</v>
       </c>
@@ -4217,7 +4237,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>660</v>
       </c>
@@ -4243,7 +4263,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>661</v>
       </c>
@@ -4269,7 +4289,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -4295,7 +4315,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -4303,6 +4323,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4314,14 +4339,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -4332,7 +4357,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -4343,7 +4368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -4357,24 +4382,34 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="2" max="2" width="41.83203125" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="13" customHeight="1">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -4393,8 +4428,11 @@
       <c r="F1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13" customHeight="1">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -4414,7 +4452,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="13" customHeight="1">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -4434,7 +4472,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="13" customHeight="1">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -4454,7 +4492,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="13" customHeight="1">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -4474,7 +4512,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="13" customHeight="1">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -4494,7 +4532,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="17">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -4514,7 +4552,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="17">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -4534,7 +4572,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -4554,7 +4592,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="17">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -4574,7 +4612,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="13.75" customHeight="1">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -4594,7 +4632,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="13.75" customHeight="1">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -4614,7 +4652,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="17">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -4634,7 +4672,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="17">
       <c r="A14" t="s">
         <v>175</v>
       </c>
@@ -4654,7 +4692,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="17">
       <c r="A15" t="s">
         <v>177</v>
       </c>
@@ -4674,7 +4712,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17">
       <c r="A16" t="s">
         <v>179</v>
       </c>
@@ -4694,7 +4732,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="17">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -4714,7 +4752,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="17">
       <c r="A18" t="s">
         <v>183</v>
       </c>
@@ -4734,7 +4772,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="17">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -4754,7 +4792,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="17">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -4774,7 +4812,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="17">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -4794,7 +4832,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="17">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -4814,7 +4852,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="17">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -4834,7 +4872,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="17">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -4854,7 +4892,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="17">
       <c r="A25" t="s">
         <v>197</v>
       </c>
@@ -4874,7 +4912,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="17">
       <c r="A26" t="s">
         <v>199</v>
       </c>
@@ -4894,7 +4932,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="17">
       <c r="A27" t="s">
         <v>201</v>
       </c>
@@ -4914,7 +4952,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="28.25" customHeight="1">
       <c r="A28" t="s">
         <v>203</v>
       </c>
@@ -4926,7 +4964,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="17">
       <c r="A29" t="s">
         <v>205</v>
       </c>
@@ -4938,7 +4976,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="17">
       <c r="A30" t="s">
         <v>207</v>
       </c>
@@ -4958,7 +4996,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="17">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -4978,13 +5016,13 @@
         <v>485</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="17">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="17">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -5004,7 +5042,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="17">
       <c r="A34" t="s">
         <v>213</v>
       </c>
@@ -5024,7 +5062,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="17">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -5044,7 +5082,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="157">
       <c r="A36" t="s">
         <v>217</v>
       </c>
@@ -5056,7 +5094,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="17">
       <c r="A37" t="s">
         <v>219</v>
       </c>
@@ -5076,7 +5114,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="17">
       <c r="A38" t="s">
         <v>221</v>
       </c>
@@ -5096,7 +5134,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="17">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5116,7 +5154,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="17">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5136,7 +5174,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="17">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5156,7 +5194,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="17">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5176,7 +5214,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="17">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5196,7 +5234,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="17">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5216,7 +5254,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="17">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5236,7 +5274,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="17">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5256,7 +5294,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="17">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5276,7 +5314,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="17">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5296,7 +5334,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="17">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5316,7 +5354,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="13" customHeight="1">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -5336,7 +5374,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="17">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -5356,7 +5394,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="17">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -5376,7 +5414,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="17">
       <c r="A53" t="s">
         <v>250</v>
       </c>
@@ -5396,7 +5434,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="17">
       <c r="A54" t="s">
         <v>252</v>
       </c>
@@ -5416,7 +5454,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="17">
       <c r="A55" s="10" t="s">
         <v>677</v>
       </c>
@@ -5431,7 +5469,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="17">
       <c r="A56" s="10" t="s">
         <v>678</v>
       </c>
@@ -5446,7 +5484,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="17">
       <c r="A57" s="10" t="s">
         <v>680</v>
       </c>
@@ -5461,52 +5499,66 @@
         <v>684</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="17">
+      <c r="A58" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>688</v>
+      </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
-    </row>
-    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="G58" s="10" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17">
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="17">
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="17">
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="17">
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="17">
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="17">
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" spans="3:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:4" ht="17">
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
     </row>
-    <row r="66" spans="3:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:4" ht="17">
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" spans="3:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:4" ht="17">
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
     </row>
-    <row r="68" spans="3:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:4" ht="17">
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved detail screens and translations
</commit_message>
<xml_diff>
--- a/appGreece/config/assets/framework/forms/framework/framework.xlsx
+++ b/appGreece/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/assets/framework/forms/framework/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="2560" windowWidth="29580" windowHeight="19960" tabRatio="989" activeTab="5"/>
+    <workbookView xWindow="3520" yWindow="1260" windowWidth="27160" windowHeight="26060" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -14,13 +19,13 @@
     <sheet name="choices" sheetId="5" r:id="rId5"/>
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="706">
   <si>
     <t>comments</t>
   </si>
@@ -929,9 +934,6 @@
     <t>Código de barras no disponible</t>
   </si>
   <si>
-    <t>Scanned beneficiary already qualifies for this distribution</t>
-  </si>
-  <si>
     <t>المستفيد متاح للتوزيع</t>
   </si>
   <si>
@@ -2057,12 +2059,6 @@
     <t>Disabled Households</t>
   </si>
   <si>
-    <t>household_data</t>
-  </si>
-  <si>
-    <t>Household Data</t>
-  </si>
-  <si>
     <t>search_members</t>
   </si>
   <si>
@@ -2105,10 +2101,70 @@
     <t>Αναμενόμενη τιμή ακέραιας</t>
   </si>
   <si>
-    <t>select_group</t>
-  </si>
-  <si>
-    <t>Please Select Group</t>
+    <t>delivery_site</t>
+  </si>
+  <si>
+    <t>household_size</t>
+  </si>
+  <si>
+    <t>tent_caravan</t>
+  </si>
+  <si>
+    <t>Delivery Site</t>
+  </si>
+  <si>
+    <t>Household Size</t>
+  </si>
+  <si>
+    <t>Tent/Caravan Code</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>household_head</t>
+  </si>
+  <si>
+    <t>vulnerability</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Household Head</t>
+  </si>
+  <si>
+    <t>Vulnerability Critieria</t>
+  </si>
+  <si>
+    <t>view_registration_data</t>
+  </si>
+  <si>
+    <t>View Registration Data</t>
+  </si>
+  <si>
+    <t>registration_data</t>
+  </si>
+  <si>
+    <t>Registration Data</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>households</t>
+  </si>
+  <si>
+    <t>search_households_title</t>
+  </si>
+  <si>
+    <t>Search for Households</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>View</t>
   </si>
 </sst>
 </file>
@@ -2171,10 +2227,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2205,13 +2259,11 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2547,7 +2599,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2561,9 +2613,9 @@
       <selection activeCell="B23" activeCellId="1" sqref="B87 B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2571,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2579,11 +2631,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2595,7 +2642,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
@@ -2606,7 +2653,7 @@
     <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2633,7 +2680,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1">
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -2642,7 +2689,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -2653,13 +2700,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -2670,23 +2717,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>255</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
         <v>256</v>
@@ -2698,20 +2745,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
         <v>257</v>
@@ -2723,7 +2770,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" t="s">
@@ -2733,433 +2780,377 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41:I41"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="3" width="49.5" customWidth="1"/>
-    <col min="4" max="4" width="62.1640625" style="5" customWidth="1"/>
-    <col min="5" max="7" width="8.83203125" style="5"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="3" max="3" width="62.1640625" style="5" customWidth="1"/>
+    <col min="4" max="6" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
-        <v>141</v>
+      <c r="C1" s="5" t="s">
+        <v>653</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>654</v>
-      </c>
-      <c r="E1" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>551</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>552</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
-        <v>27</v>
+      <c r="C2" s="5" t="s">
+        <v>552</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>553</v>
+        <v>260</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="G2" s="5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
+      <c r="C3" s="5" t="s">
+        <v>553</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>554</v>
+        <v>263</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="G3" s="5" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
-        <v>31</v>
+      <c r="C4" s="5" t="s">
+        <v>554</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>555</v>
+        <v>266</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="G4" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="C5" t="s">
-        <v>34</v>
+      <c r="C5" s="5" t="s">
+        <v>555</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>556</v>
+        <v>268</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="G5" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
-        <v>37</v>
+      <c r="C6" s="5" t="s">
+        <v>556</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>557</v>
+        <v>270</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="G6" s="5" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
-        <v>39</v>
+      <c r="C7" s="5" t="s">
+        <v>557</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>558</v>
+        <v>273</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="G7" s="5" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" t="s">
-        <v>41</v>
+      <c r="C8" s="5" t="s">
+        <v>558</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>559</v>
+        <v>276</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G8" s="5" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
+      <c r="C9" s="5" t="s">
+        <v>559</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>560</v>
+        <v>279</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="G9" s="5" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
-        <v>45</v>
+      <c r="C10" s="5" t="s">
+        <v>560</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>561</v>
+        <v>282</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="G10" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
       <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
-        <v>48</v>
+      <c r="C11" s="5" t="s">
+        <v>561</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>562</v>
+        <v>284</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="G11" s="5" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
-        <v>50</v>
+      <c r="C12" s="5" t="s">
+        <v>562</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>563</v>
+        <v>287</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="G12" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
-        <v>52</v>
+      <c r="C13" s="5" t="s">
+        <v>563</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>564</v>
+        <v>290</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="G13" s="5" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>53</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" t="s">
-        <v>54</v>
+      <c r="C14" s="5" t="s">
+        <v>564</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>565</v>
+        <v>293</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="G14" s="5" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="34">
+    <row r="15" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>566</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>58</v>
       </c>
-      <c r="C16" t="s">
-        <v>58</v>
+      <c r="C16" s="5" t="s">
+        <v>566</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>567</v>
+        <v>298</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>568</v>
+      <c r="C17" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>301</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>61</v>
       </c>
       <c r="B18" t="s">
+        <v>304</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>568</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="C18" t="s">
-        <v>305</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>569</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>306</v>
@@ -3167,22 +3158,19 @@
       <c r="F18" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s">
-        <v>63</v>
+      <c r="C19" s="5" t="s">
+        <v>569</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>570</v>
+        <v>308</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>309</v>
@@ -3190,22 +3178,19 @@
       <c r="F19" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
-        <v>65</v>
+      <c r="C20" s="5" t="s">
+        <v>570</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>571</v>
+        <v>311</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>312</v>
@@ -3213,22 +3198,19 @@
       <c r="F20" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>67</v>
       </c>
-      <c r="C21" t="s">
-        <v>67</v>
+      <c r="C21" s="5" t="s">
+        <v>571</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>572</v>
+        <v>314</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>315</v>
@@ -3236,22 +3218,19 @@
       <c r="F21" s="5" t="s">
         <v>316</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" t="s">
-        <v>69</v>
+      <c r="C22" s="5" t="s">
+        <v>572</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>573</v>
+        <v>317</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>318</v>
@@ -3259,22 +3238,19 @@
       <c r="F22" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
-        <v>71</v>
+      <c r="C23" s="5" t="s">
+        <v>573</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>574</v>
+        <v>320</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>321</v>
@@ -3282,22 +3258,19 @@
       <c r="F23" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>72</v>
       </c>
       <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
-        <v>73</v>
+      <c r="C24" s="5" t="s">
+        <v>574</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>575</v>
+        <v>323</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>324</v>
@@ -3305,22 +3278,19 @@
       <c r="F24" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
       <c r="B25" t="s">
         <v>75</v>
       </c>
-      <c r="C25" t="s">
-        <v>75</v>
+      <c r="C25" s="5" t="s">
+        <v>575</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>576</v>
+        <v>326</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>327</v>
@@ -3328,22 +3298,19 @@
       <c r="F25" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>76</v>
       </c>
       <c r="B26" t="s">
         <v>77</v>
       </c>
-      <c r="C26" t="s">
-        <v>77</v>
+      <c r="C26" s="5" t="s">
+        <v>576</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>577</v>
+        <v>329</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>330</v>
@@ -3351,22 +3318,19 @@
       <c r="F26" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
       <c r="B27" t="s">
         <v>79</v>
       </c>
-      <c r="C27" t="s">
-        <v>79</v>
+      <c r="C27" s="5" t="s">
+        <v>577</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>578</v>
+        <v>332</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>333</v>
@@ -3374,22 +3338,19 @@
       <c r="F27" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>80</v>
       </c>
       <c r="B28" t="s">
         <v>81</v>
       </c>
-      <c r="C28" t="s">
-        <v>81</v>
+      <c r="C28" s="5" t="s">
+        <v>578</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>579</v>
+        <v>335</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>336</v>
@@ -3397,22 +3358,19 @@
       <c r="F28" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
       <c r="B29" t="s">
         <v>83</v>
       </c>
-      <c r="C29" t="s">
-        <v>83</v>
+      <c r="C29" s="5" t="s">
+        <v>579</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>580</v>
+        <v>338</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>339</v>
@@ -3420,22 +3378,19 @@
       <c r="F29" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>84</v>
       </c>
       <c r="B30" t="s">
         <v>85</v>
       </c>
-      <c r="C30" t="s">
-        <v>85</v>
+      <c r="C30" s="5" t="s">
+        <v>580</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>581</v>
+        <v>341</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>342</v>
@@ -3443,45 +3398,39 @@
       <c r="F30" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>86</v>
       </c>
       <c r="B31" t="s">
         <v>87</v>
       </c>
-      <c r="C31" t="s">
-        <v>87</v>
+      <c r="C31" s="5" t="s">
+        <v>581</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>582</v>
+        <v>344</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="G31" s="8" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>88</v>
       </c>
       <c r="B32" t="s">
         <v>89</v>
       </c>
-      <c r="C32" t="s">
-        <v>89</v>
+      <c r="C32" s="5" t="s">
+        <v>582</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>583</v>
+        <v>347</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>348</v>
@@ -3489,22 +3438,19 @@
       <c r="F32" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
       <c r="B33" t="s">
         <v>91</v>
       </c>
-      <c r="C33" t="s">
-        <v>91</v>
+      <c r="C33" s="5" t="s">
+        <v>583</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>584</v>
+        <v>350</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>351</v>
@@ -3512,22 +3458,19 @@
       <c r="F33" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>92</v>
       </c>
       <c r="B34" t="s">
         <v>93</v>
       </c>
-      <c r="C34" t="s">
-        <v>93</v>
+      <c r="C34" s="5" t="s">
+        <v>584</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>585</v>
+        <v>353</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>354</v>
@@ -3535,22 +3478,19 @@
       <c r="F34" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>94</v>
       </c>
       <c r="B35" t="s">
         <v>95</v>
       </c>
-      <c r="C35" t="s">
-        <v>95</v>
+      <c r="C35" s="5" t="s">
+        <v>585</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>586</v>
+        <v>356</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>357</v>
@@ -3558,22 +3498,19 @@
       <c r="F35" s="5" t="s">
         <v>358</v>
       </c>
-      <c r="G35" s="5" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>96</v>
       </c>
       <c r="B36" t="s">
         <v>97</v>
       </c>
-      <c r="C36" t="s">
-        <v>97</v>
+      <c r="C36" s="5" t="s">
+        <v>586</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>587</v>
+        <v>359</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>360</v>
@@ -3581,22 +3518,19 @@
       <c r="F36" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>98</v>
       </c>
       <c r="B37" t="s">
         <v>99</v>
       </c>
-      <c r="C37" t="s">
-        <v>99</v>
+      <c r="C37" s="5" t="s">
+        <v>587</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>588</v>
+        <v>362</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>363</v>
@@ -3604,22 +3538,19 @@
       <c r="F37" s="5" t="s">
         <v>364</v>
       </c>
-      <c r="G37" s="5" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>100</v>
       </c>
       <c r="B38" t="s">
         <v>101</v>
       </c>
-      <c r="C38" t="s">
-        <v>101</v>
+      <c r="C38" s="5" t="s">
+        <v>588</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>589</v>
+        <v>365</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>366</v>
@@ -3627,22 +3558,19 @@
       <c r="F38" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="G38" s="5" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>102</v>
       </c>
       <c r="B39" t="s">
         <v>103</v>
       </c>
-      <c r="C39" t="s">
-        <v>103</v>
+      <c r="C39" s="5" t="s">
+        <v>589</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>590</v>
+        <v>368</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>369</v>
@@ -3650,22 +3578,19 @@
       <c r="F39" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>259</v>
       </c>
       <c r="B40" t="s">
         <v>104</v>
       </c>
-      <c r="C40" t="s">
-        <v>104</v>
+      <c r="C40" s="5" t="s">
+        <v>590</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>591</v>
+        <v>371</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>372</v>
@@ -3673,22 +3598,19 @@
       <c r="F40" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>105</v>
       </c>
       <c r="B41" t="s">
         <v>106</v>
       </c>
-      <c r="C41" t="s">
-        <v>106</v>
+      <c r="C41" s="5" t="s">
+        <v>591</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>592</v>
+        <v>374</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>375</v>
@@ -3696,22 +3618,19 @@
       <c r="F41" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="G41" s="5" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>107</v>
       </c>
       <c r="B42" t="s">
         <v>107</v>
       </c>
-      <c r="C42" t="s">
-        <v>107</v>
+      <c r="C42" s="5" t="s">
+        <v>592</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>593</v>
+        <v>377</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>378</v>
@@ -3719,91 +3638,79 @@
       <c r="F42" s="5" t="s">
         <v>379</v>
       </c>
-      <c r="G42" s="5" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>108</v>
       </c>
       <c r="B43" t="s">
         <v>108</v>
       </c>
-      <c r="C43" t="s">
-        <v>108</v>
+      <c r="C43" s="5" t="s">
+        <v>593</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>594</v>
+        <v>380</v>
       </c>
       <c r="E43" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>109</v>
       </c>
       <c r="B44" t="s">
         <v>109</v>
       </c>
-      <c r="C44" t="s">
-        <v>109</v>
+      <c r="C44" s="5" t="s">
+        <v>594</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>595</v>
+        <v>382</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>383</v>
+        <v>269</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="G44" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>110</v>
       </c>
       <c r="B45" t="s">
         <v>110</v>
       </c>
-      <c r="C45" t="s">
-        <v>110</v>
+      <c r="C45" s="5" t="s">
+        <v>595</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>596</v>
+        <v>383</v>
       </c>
       <c r="E45" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>111</v>
       </c>
       <c r="B46" t="s">
         <v>111</v>
       </c>
-      <c r="C46" t="s">
-        <v>111</v>
+      <c r="C46" s="5" t="s">
+        <v>596</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>597</v>
+        <v>385</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>386</v>
@@ -3811,22 +3718,19 @@
       <c r="F46" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>112</v>
       </c>
       <c r="B47" t="s">
         <v>113</v>
       </c>
-      <c r="C47" t="s">
-        <v>113</v>
+      <c r="C47" s="5" t="s">
+        <v>597</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>598</v>
+        <v>388</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>389</v>
@@ -3834,22 +3738,19 @@
       <c r="F47" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="G47" s="5" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>392</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>599</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>393</v>
@@ -3857,45 +3758,39 @@
       <c r="F48" s="5" t="s">
         <v>394</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="C49" s="5" t="s">
-        <v>396</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>600</v>
-      </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>117</v>
+      <c r="C50" s="5" t="s">
+        <v>600</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>601</v>
+        <v>399</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>400</v>
@@ -3903,68 +3798,59 @@
       <c r="F50" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="G50" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="34">
+    </row>
+    <row r="51" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>119</v>
+      <c r="C51" s="5" t="s">
+        <v>601</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>602</v>
-      </c>
-      <c r="E51" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="G51" s="5" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>121</v>
+      <c r="C52" s="5" t="s">
+        <v>602</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>603</v>
-      </c>
-      <c r="E52" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E52" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="G52" s="5" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="2" customFormat="1">
+    </row>
+    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>123</v>
+      <c r="C53" s="5" t="s">
+        <v>603</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>604</v>
+        <v>408</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>409</v>
@@ -3972,91 +3858,167 @@
       <c r="F53" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="G53" s="5" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>253</v>
       </c>
       <c r="B54" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>604</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>412</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>605</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="F54" s="5" t="s">
+      <c r="F54" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="G54" s="8" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="G55" s="8"/>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="B56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>669</v>
       </c>
-      <c r="B57" s="2" t="s">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="2" t="s">
+      <c r="B62" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="2" t="s">
-        <v>674</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>676</v>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>690</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>691</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>692</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>696</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>704</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>705</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4068,9 +4030,9 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>124</v>
       </c>
@@ -4084,13 +4046,13 @@
         <v>127</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>663</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>664</v>
       </c>
       <c r="H1" t="s">
         <v>128</v>
@@ -4099,13 +4061,13 @@
         <v>129</v>
       </c>
       <c r="J1" t="s">
+        <v>654</v>
+      </c>
+      <c r="K1" t="s">
         <v>655</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>656</v>
-      </c>
-      <c r="L1" t="s">
-        <v>657</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -4114,7 +4076,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>131</v>
       </c>
@@ -4132,7 +4094,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>133</v>
       </c>
@@ -4153,7 +4115,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
@@ -4164,7 +4126,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28" customHeight="1">
+    <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -4191,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -4211,7 +4173,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>143</v>
       </c>
@@ -4237,9 +4199,9 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4248,24 +4210,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4274,22 +4236,22 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -4315,7 +4277,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>254</v>
       </c>
@@ -4323,11 +4285,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4339,14 +4296,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>148</v>
       </c>
@@ -4357,7 +4314,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -4368,7 +4325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -4382,34 +4339,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="2" max="2" width="41.83203125" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="36.33203125" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1">
+    <row r="1" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -4417,22 +4364,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E1" t="s">
         <v>551</v>
-      </c>
-      <c r="E1" t="s">
-        <v>552</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1">
+    </row>
+    <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>151</v>
       </c>
@@ -4440,19 +4384,19 @@
         <v>152</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="8" t="s">
         <v>417</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="13" customHeight="1">
+    </row>
+    <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>153</v>
       </c>
@@ -4460,19 +4404,19 @@
         <v>154</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="13" customHeight="1">
+    </row>
+    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -4480,19 +4424,19 @@
         <v>156</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="13" customHeight="1">
+    </row>
+    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -4500,19 +4444,19 @@
         <v>158</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="13" customHeight="1">
+    </row>
+    <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -4520,19 +4464,19 @@
         <v>160</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="17">
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -4540,19 +4484,19 @@
         <v>162</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="17">
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -4560,19 +4504,19 @@
         <v>164</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="17">
+    </row>
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -4580,19 +4524,19 @@
         <v>166</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="17">
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -4600,19 +4544,19 @@
         <v>168</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>440</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="13.75" customHeight="1">
+    </row>
+    <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -4620,19 +4564,19 @@
         <v>170</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="13.75" customHeight="1">
+    </row>
+    <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -4640,19 +4584,19 @@
         <v>172</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>423</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17">
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>173</v>
       </c>
@@ -4660,19 +4604,19 @@
         <v>174</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>446</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="17">
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>175</v>
       </c>
@@ -4680,19 +4624,19 @@
         <v>176</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>540</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17">
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>177</v>
       </c>
@@ -4700,19 +4644,19 @@
         <v>178</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>544</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>545</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17">
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>179</v>
       </c>
@@ -4720,19 +4664,19 @@
         <v>180</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>547</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>548</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>181</v>
       </c>
@@ -4740,19 +4684,19 @@
         <v>182</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>549</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>550</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>183</v>
       </c>
@@ -4760,19 +4704,19 @@
         <v>184</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="17">
+    </row>
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -4780,19 +4724,19 @@
         <v>186</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="17">
+    </row>
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>187</v>
       </c>
@@ -4800,19 +4744,19 @@
         <v>188</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17">
+    </row>
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>189</v>
       </c>
@@ -4820,19 +4764,19 @@
         <v>190</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="17">
+    </row>
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -4840,19 +4784,19 @@
         <v>192</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>463</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="17">
+    </row>
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -4860,19 +4804,19 @@
         <v>194</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17">
+    </row>
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -4880,19 +4824,19 @@
         <v>196</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>470</v>
       </c>
-      <c r="F24" s="5" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="17">
+    </row>
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>197</v>
       </c>
@@ -4900,19 +4844,19 @@
         <v>198</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>472</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>473</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17">
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>199</v>
       </c>
@@ -4920,19 +4864,19 @@
         <v>200</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="F26" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="17">
+    </row>
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>201</v>
       </c>
@@ -4940,19 +4884,19 @@
         <v>202</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="28.25" customHeight="1">
+    </row>
+    <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>203</v>
       </c>
@@ -4964,7 +4908,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="17">
+    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>205</v>
       </c>
@@ -4976,7 +4920,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="17">
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>207</v>
       </c>
@@ -4984,19 +4928,19 @@
         <v>208</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="F30" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17">
+    </row>
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -5004,25 +4948,25 @@
         <v>210</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17">
+    </row>
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="17">
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>211</v>
       </c>
@@ -5030,19 +4974,19 @@
         <v>212</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>486</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="F33" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="17">
+    </row>
+    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>213</v>
       </c>
@@ -5050,19 +4994,19 @@
         <v>214</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="17">
+    </row>
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>215</v>
       </c>
@@ -5070,19 +5014,19 @@
         <v>216</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>492</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="F35" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="F35" s="8" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="157">
+    </row>
+    <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>217</v>
       </c>
@@ -5094,7 +5038,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="17">
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>219</v>
       </c>
@@ -5102,19 +5046,19 @@
         <v>220</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>495</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="F37" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="17">
+    </row>
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>221</v>
       </c>
@@ -5122,19 +5066,19 @@
         <v>222</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>498</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>499</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="17">
+    </row>
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>223</v>
       </c>
@@ -5142,19 +5086,19 @@
         <v>224</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>501</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="F39" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="17">
+    </row>
+    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>225</v>
       </c>
@@ -5162,19 +5106,19 @@
         <v>226</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>504</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="F40" s="5" t="s">
         <v>505</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="17">
+    </row>
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>227</v>
       </c>
@@ -5182,19 +5126,19 @@
         <v>228</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D41" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="F41" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="17">
+    </row>
+    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>229</v>
       </c>
@@ -5202,19 +5146,19 @@
         <v>230</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>510</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="F42" s="5" t="s">
         <v>511</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="17">
+    </row>
+    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>231</v>
       </c>
@@ -5222,19 +5166,19 @@
         <v>232</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>513</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>514</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17">
+    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>233</v>
       </c>
@@ -5242,19 +5186,19 @@
         <v>234</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="F44" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="17">
+    </row>
+    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -5262,19 +5206,19 @@
         <v>236</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D45" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>518</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="F45" s="5" t="s">
         <v>519</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="17">
+    </row>
+    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>237</v>
       </c>
@@ -5282,19 +5226,19 @@
         <v>238</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D46" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>521</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="F46" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="F46" s="5" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="17">
+    </row>
+    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>239</v>
       </c>
@@ -5302,19 +5246,19 @@
         <v>240</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D47" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="F47" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="F47" s="5" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="17">
+    </row>
+    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>241</v>
       </c>
@@ -5322,19 +5266,19 @@
         <v>242</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D48" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="F48" s="5" t="s">
         <v>528</v>
       </c>
-      <c r="F48" s="5" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="17">
+    </row>
+    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>243</v>
       </c>
@@ -5342,19 +5286,19 @@
         <v>244</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>530</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="F49" s="5" t="s">
         <v>531</v>
       </c>
-      <c r="F49" s="5" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="13" customHeight="1">
+    </row>
+    <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>245</v>
       </c>
@@ -5362,19 +5306,19 @@
         <v>246</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>533</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="F50" s="5" t="s">
         <v>534</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="17">
+    </row>
+    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>247</v>
       </c>
@@ -5382,19 +5326,19 @@
         <v>248</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="F51" s="5" t="s">
         <v>536</v>
       </c>
-      <c r="E51" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="17">
+    </row>
+    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>249</v>
       </c>
@@ -5402,19 +5346,19 @@
         <v>210</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>483</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="F52" s="5" t="s">
         <v>484</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="17">
+    </row>
+    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>250</v>
       </c>
@@ -5422,19 +5366,19 @@
         <v>251</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="F53" s="5" t="s">
         <v>539</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="17">
+    </row>
+    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>252</v>
       </c>
@@ -5442,21 +5386,21 @@
         <v>240</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D54" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="F54" s="5" t="s">
         <v>525</v>
       </c>
-      <c r="F54" s="5" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="17">
+    </row>
+    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>63</v>
@@ -5466,99 +5410,85 @@
       </c>
       <c r="D55" s="5"/>
       <c r="F55" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>682</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="17">
-      <c r="A56" s="10" t="s">
-        <v>678</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>679</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>685</v>
       </c>
       <c r="D56" s="5"/>
       <c r="F56" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="17">
-      <c r="A57" s="10" t="s">
-        <v>680</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>681</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>686</v>
       </c>
       <c r="D57" s="5"/>
       <c r="F57" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="17">
-      <c r="A58" s="10" t="s">
-        <v>687</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>688</v>
-      </c>
+        <v>681</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
-      <c r="G58" s="10" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="17">
+    </row>
+    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
     </row>
-    <row r="60" spans="1:7" ht="17">
+    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
     </row>
-    <row r="61" spans="1:7" ht="17">
+    <row r="61" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
     </row>
-    <row r="62" spans="1:7" ht="17">
+    <row r="62" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
     </row>
-    <row r="63" spans="1:7" ht="17">
+    <row r="63" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
     </row>
-    <row r="64" spans="1:7" ht="17">
+    <row r="64" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" spans="3:4" ht="17">
+    <row r="65" spans="3:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
     </row>
-    <row r="66" spans="3:4" ht="17">
+    <row r="66" spans="3:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" spans="3:4" ht="17">
+    <row r="67" spans="3:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
     </row>
-    <row r="68" spans="3:4" ht="17">
+    <row r="68" spans="3:4" ht="18" x14ac:dyDescent="0.2">
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>